<commit_message>
modify code and run for second time
</commit_message>
<xml_diff>
--- a/comparison_results.xlsx
+++ b/comparison_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9472868217054263</v>
+        <v>0.9410852713178295</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9254385964912281</v>
+        <v>0.9122807017543859</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9254385964912281</v>
+        <v>0.9203539823008849</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9254385964912281</v>
+        <v>0.9162995594713657</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9395348837209302</v>
+        <v>0.9441860465116279</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9122807017543859</v>
+        <v>0.9298245614035088</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9162995594713657</v>
+        <v>0.9137931034482759</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9142857142857143</v>
+        <v>0.9217391304347826</v>
       </c>
     </row>
     <row r="4">
@@ -558,38 +558,57 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ExtraTrees</t>
+          <t>LightGBM</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8573643410852713</v>
+        <v>0.9488372093023256</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7149122807017544</v>
+        <v>0.9254385964912281</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8578947368421053</v>
+        <v>0.9295154185022027</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7799043062200957</v>
+        <v>0.9274725274725275</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>ExtraTrees</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8527131782945736</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6885964912280702</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8674033149171271</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.7677261613691931</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>GradientBoosting</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B9" t="n">
         <v>0.951937984496124</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C9" t="n">
         <v>0.9342105263157895</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>0.9301310043668122</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" t="n">
         <v>0.9321663019693655</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add codes to jupyter notebook
</commit_message>
<xml_diff>
--- a/comparison_results.xlsx
+++ b/comparison_results.xlsx
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9410852713178295</v>
+        <v>0.9457364341085271</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9122807017543859</v>
+        <v>0.9298245614035088</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9203539823008849</v>
+        <v>0.9177489177489178</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9162995594713657</v>
+        <v>0.9237472766884531</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9441860465116279</v>
+        <v>0.9364341085271318</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9298245614035088</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9137931034482759</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9217391304347826</v>
+        <v>0.9106753812636166</v>
       </c>
     </row>
     <row r="4">
@@ -581,16 +581,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8527131782945736</v>
+        <v>0.8682170542635659</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6885964912280702</v>
+        <v>0.7280701754385965</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8674033149171271</v>
+        <v>0.8783068783068783</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7677261613691931</v>
+        <v>0.7961630695443646</v>
       </c>
     </row>
     <row r="9">

</xml_diff>